<commit_message>
plan de proyecto corregido
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1366 - RNCNOM, Gabriela de la Torre_MO/Planeación/Plan_proyecto.xlsx
+++ b/Proyectos/2015/12/P1366 - RNCNOM, Gabriela de la Torre_MO/Planeación/Plan_proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="166">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Proporcionar conexión y realizar el pago del servicio</t>
-  </si>
-  <si>
     <t>Estructura Organizacional</t>
   </si>
   <si>
@@ -636,15 +633,6 @@
   </si>
   <si>
     <t>Alto</t>
-  </si>
-  <si>
-    <t>Mario Govea</t>
-  </si>
-  <si>
-    <t>callto:5555124630</t>
-  </si>
-  <si>
-    <t>mayo956@hotmail.com</t>
   </si>
   <si>
     <t>P1358 - RNCFAC, Carlos Mendoza, Oscar Daniel_MO</t>
@@ -2043,7 +2031,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="147" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C3" s="147"/>
     </row>
@@ -4201,7 +4189,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="145" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:1023" ht="12.75" customHeight="1">
@@ -4397,7 +4385,7 @@
     </row>
     <row r="26" spans="1:4" ht="53.65" customHeight="1">
       <c r="A26" s="153" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B26" s="153"/>
       <c r="C26" s="10"/>
@@ -4410,7 +4398,7 @@
     </row>
     <row r="28" spans="1:4" ht="53.25" customHeight="1">
       <c r="A28" s="150" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B28" s="151"/>
     </row>
@@ -4428,11 +4416,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
@@ -4442,6 +4425,11 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A28" r:id="rId1"/>
@@ -4455,8 +4443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4623,22 +4611,14 @@
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="25.5">
+    <row r="13" spans="1:5">
       <c r="A13" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>70</v>
-      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="29"/>
@@ -4670,7 +4650,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -4684,7 +4664,7 @@
     <row r="23" spans="1:5" ht="18.75">
       <c r="A23" s="35"/>
       <c r="B23" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4705,7 +4685,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4720,19 +4700,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="38" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5910,7 +5890,7 @@
     </row>
     <row r="2" spans="1:1023" ht="28.5" customHeight="1">
       <c r="A2" s="154" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="154"/>
       <c r="C2" s="154"/>
@@ -6937,19 +6917,19 @@
     </row>
     <row r="3" spans="1:1023">
       <c r="A3" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="C3" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="44" t="s">
         <v>81</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>82</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -7972,16 +7952,16 @@
     </row>
     <row r="4" spans="1:1023" ht="25.5">
       <c r="A4" s="45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E4" s="47"/>
       <c r="F4"/>
@@ -9005,58 +8985,58 @@
     </row>
     <row r="5" spans="1:1023" s="50" customFormat="1" ht="25.5">
       <c r="A5" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1023" s="50" customFormat="1" ht="25.5">
       <c r="A6" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1023" s="50" customFormat="1" ht="51">
       <c r="A7" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="49" t="s">
         <v>61</v>
       </c>
       <c r="C7" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="E7" s="49" t="s">
         <v>88</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1023" s="50" customFormat="1" ht="25.5">
       <c r="A8" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="E8" s="49" t="s">
         <v>92</v>
-      </c>
-      <c r="E8" s="49" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:1023" s="50" customFormat="1">
@@ -9131,7 +9111,7 @@
     </row>
     <row r="2" spans="1:10" ht="22.5" customHeight="1">
       <c r="A2" s="149" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="149"/>
       <c r="C2" s="149"/>
@@ -9143,37 +9123,37 @@
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="53" t="s">
         <v>103</v>
-      </c>
-      <c r="C4" s="53" t="s">
-        <v>104</v>
       </c>
       <c r="D4" s="31">
         <v>1</v>
@@ -9182,22 +9162,22 @@
         <v>42345</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="31"/>
       <c r="J4" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="53" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" s="53" t="s">
-        <v>104</v>
       </c>
       <c r="D5" s="31">
         <v>1</v>
@@ -9206,22 +9186,22 @@
         <v>42345</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" s="31"/>
       <c r="J5" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="51">
       <c r="A6" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="53" t="s">
-        <v>108</v>
-      </c>
       <c r="C6" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="53">
         <v>2</v>
@@ -9230,13 +9210,13 @@
         <v>42345</v>
       </c>
       <c r="F6" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9341,7 +9321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:JA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -9372,7 +9352,7 @@
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
       <c r="E2" s="62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" s="63"/>
       <c r="G2" s="63"/>
@@ -9381,7 +9361,7 @@
       <c r="J2" s="63"/>
       <c r="K2" s="64"/>
       <c r="IR2" s="65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="IS2" s="65"/>
       <c r="IT2" s="65"/>
@@ -9406,51 +9386,51 @@
       <c r="J3" s="69"/>
       <c r="K3" s="70"/>
       <c r="AE3" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF3" s="71" t="s">
         <v>112</v>
-      </c>
-      <c r="AF3" s="71" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:261" ht="30">
       <c r="A4" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="C4" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="D4" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="E4" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="F4" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="G4" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="74" t="s">
+      <c r="H4" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="74" t="s">
+      <c r="I4" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="J4" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="K4" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="K4" s="74" t="s">
-        <v>124</v>
-      </c>
       <c r="AE4" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF4" s="76" t="s">
         <v>112</v>
-      </c>
-      <c r="AF4" s="76" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:261" ht="76.5">
@@ -9458,7 +9438,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="77">
         <v>1</v>
@@ -9474,17 +9454,17 @@
         <v>4</v>
       </c>
       <c r="G5" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="78" t="s">
         <v>126</v>
-      </c>
-      <c r="H5" s="78" t="s">
-        <v>127</v>
       </c>
       <c r="I5" s="80"/>
       <c r="J5" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="82" t="s">
         <v>128</v>
-      </c>
-      <c r="K5" s="82" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:261" ht="51">
@@ -9492,7 +9472,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="77">
         <v>4</v>
@@ -9508,17 +9488,17 @@
         <v>3</v>
       </c>
       <c r="G6" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="82" t="s">
         <v>131</v>
-      </c>
-      <c r="H6" s="82" t="s">
-        <v>132</v>
       </c>
       <c r="I6" s="80"/>
       <c r="J6" s="81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:261" ht="51">
@@ -9526,7 +9506,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="77">
         <v>4</v>
@@ -9542,17 +9522,17 @@
         <v>3</v>
       </c>
       <c r="G7" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="78" t="s">
         <v>135</v>
-      </c>
-      <c r="H7" s="78" t="s">
-        <v>136</v>
       </c>
       <c r="I7" s="77"/>
       <c r="J7" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="82" t="s">
         <v>128</v>
-      </c>
-      <c r="K7" s="82" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:261" ht="38.25">
@@ -9560,7 +9540,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="77">
         <v>5</v>
@@ -9576,19 +9556,19 @@
         <v>4</v>
       </c>
       <c r="G8" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="78" t="s">
         <v>138</v>
-      </c>
-      <c r="H8" s="78" t="s">
-        <v>139</v>
       </c>
       <c r="I8" s="77" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K8" s="82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="IS8" s="83"/>
       <c r="IT8" s="84"/>
@@ -9604,7 +9584,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="77">
         <v>5</v>
@@ -9620,25 +9600,25 @@
         <v>4</v>
       </c>
       <c r="G9" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="78" t="s">
         <v>141</v>
-      </c>
-      <c r="H9" s="78" t="s">
-        <v>142</v>
       </c>
       <c r="I9" s="77" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="81" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="IS9" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="K9" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="IS9" s="88" t="s">
+      <c r="IT9" s="89" t="s">
         <v>144</v>
-      </c>
-      <c r="IT9" s="89" t="s">
-        <v>145</v>
       </c>
       <c r="IU9" s="90">
         <v>0.9</v>
@@ -9669,7 +9649,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="77">
         <v>1</v>
@@ -9685,23 +9665,23 @@
         <v>3</v>
       </c>
       <c r="G10" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" s="78" t="s">
         <v>147</v>
-      </c>
-      <c r="H10" s="78" t="s">
-        <v>148</v>
       </c>
       <c r="I10" s="77" t="s">
         <v>51</v>
       </c>
       <c r="J10" s="81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K10" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="IS10" s="88"/>
       <c r="IT10" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="IU10" s="90">
         <v>0.7</v>
@@ -9746,7 +9726,7 @@
       <c r="K11" s="104"/>
       <c r="IS11" s="88"/>
       <c r="IT11" s="89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="IU11" s="90">
         <v>0.5</v>
@@ -9791,7 +9771,7 @@
       <c r="K12" s="104"/>
       <c r="IS12" s="88"/>
       <c r="IT12" s="89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="IU12" s="90">
         <v>0.3</v>
@@ -9836,7 +9816,7 @@
       <c r="K13" s="104"/>
       <c r="IS13" s="88"/>
       <c r="IT13" s="89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="IU13" s="111">
         <v>0.1</v>
@@ -9919,19 +9899,19 @@
       <c r="IT15" s="124"/>
       <c r="IU15" s="124"/>
       <c r="IV15" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="IW15" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="IW15" s="89" t="s">
+      <c r="IX15" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="IX15" s="89" t="s">
-        <v>153</v>
-      </c>
       <c r="IY15" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="IZ15" s="126" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:261" ht="15">
@@ -9955,7 +9935,7 @@
       <c r="IT16" s="124"/>
       <c r="IU16" s="90"/>
       <c r="IV16" s="127" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="IW16" s="127"/>
       <c r="IX16" s="127"/>
@@ -10032,7 +10012,7 @@
       <c r="J19" s="121"/>
       <c r="K19" s="122"/>
       <c r="IS19" s="131" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="IT19" s="131"/>
       <c r="IU19" s="129"/>
@@ -10060,12 +10040,12 @@
       <c r="J20" s="121"/>
       <c r="K20" s="122"/>
       <c r="IS20" s="132" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="IT20" s="133"/>
       <c r="IU20" s="129"/>
       <c r="IV20" s="134" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="IW20" s="134"/>
       <c r="IX20" s="134"/>
@@ -10090,12 +10070,12 @@
       <c r="J21" s="121"/>
       <c r="K21" s="122"/>
       <c r="IS21" s="132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="IT21" s="135"/>
       <c r="IU21" s="129"/>
       <c r="IV21" s="134" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="IW21" s="134"/>
       <c r="IX21" s="134"/>
@@ -10120,12 +10100,12 @@
       <c r="J22" s="121"/>
       <c r="K22" s="122"/>
       <c r="IS22" s="132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="IT22" s="136"/>
       <c r="IU22" s="129"/>
       <c r="IV22" s="134" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="IW22" s="134"/>
       <c r="IX22" s="134"/>

</xml_diff>